<commit_message>
I don't even know how to name commits
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" calcOnSave="0"/>
 </workbook>
 </file>
 
@@ -765,8 +765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BW20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="50.1" customHeight="1"/>

</xml_diff>